<commit_message>
Urenverdeling Week 1 Afgemaakt
</commit_message>
<xml_diff>
--- a/Urenverdeling Week1.xlsx
+++ b/Urenverdeling Week1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t xml:space="preserve">Planning van de uren </t>
   </si>
@@ -111,6 +111,45 @@
   </si>
   <si>
     <t>Dag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robot de lijn laten volgen </t>
+  </si>
+  <si>
+    <t>Geluid met robot uitzoeken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De robot laten stoppen bij een object </t>
+  </si>
+  <si>
+    <t>De robot laten stoppen bij een kruising</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bluethooth verbinden </t>
+  </si>
+  <si>
+    <t xml:space="preserve">De robot geluid laten maken </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Via bluetooth de robot besturen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geluid afspelen tijdens het rijden </t>
+  </si>
+  <si>
+    <t>Robot kan lijn volgen</t>
+  </si>
+  <si>
+    <t>Bluetooth verbinding</t>
+  </si>
+  <si>
+    <t>Robot kruising</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>15 min.</t>
   </si>
 </sst>
 </file>
@@ -142,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,12 +226,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -379,21 +412,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -405,10 +429,41 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -429,44 +484,23 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -752,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,83 +805,84 @@
     <col min="19" max="19" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="12"/>
+    <row r="1" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="9"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="35"/>
-      <c r="D2" s="15" t="s">
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="D2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="38"/>
+      <c r="F2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19" t="s">
+      <c r="G2" s="40"/>
+      <c r="H2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="13" t="s">
+      <c r="I2" s="42"/>
+      <c r="J2" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="14"/>
+      <c r="K2" s="44"/>
       <c r="M2" s="2"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:19" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="1:20" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-    </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="36">
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+    </row>
+    <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="22">
         <v>42450</v>
       </c>
       <c r="C4" t="s">
@@ -877,32 +912,32 @@
       <c r="K4" s="1">
         <v>1</v>
       </c>
-      <c r="L4" s="31"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="49" t="s">
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="50" t="s">
+      <c r="O4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" s="53" t="s">
+      <c r="Q4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="51" t="s">
+      <c r="R4" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="S4" s="54" t="s">
+      <c r="S4" s="33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="36">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="22">
         <v>42450</v>
       </c>
       <c r="C5" t="s">
@@ -932,32 +967,32 @@
       <c r="K5" s="1">
         <v>0.5</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="47">
+      <c r="L5" s="15"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="26">
         <v>42450</v>
       </c>
-      <c r="O5" s="46" t="s">
+      <c r="O5" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="46" t="s">
+      <c r="P5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="46" t="s">
+      <c r="Q5" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="R5" s="46" t="s">
+      <c r="R5" s="25" t="s">
         <v>23</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="36">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="22">
         <v>42450</v>
       </c>
       <c r="C6" t="s">
@@ -987,20 +1022,32 @@
       <c r="K6" s="1">
         <v>0</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" s="36">
+      <c r="L6" s="15"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="26">
+        <v>42451</v>
+      </c>
+      <c r="O6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="22">
         <v>42450</v>
       </c>
       <c r="C7" t="s">
@@ -1030,20 +1077,32 @@
       <c r="K7" s="1">
         <v>0</v>
       </c>
-      <c r="L7" s="27"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
-      <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="36">
+      <c r="L7" s="15"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="26">
+        <v>42452</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="22">
         <v>42450</v>
       </c>
       <c r="C8" t="s">
@@ -1073,20 +1132,32 @@
       <c r="K8" s="1">
         <v>2</v>
       </c>
-      <c r="L8" s="27"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="36">
+      <c r="L8" s="15"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="54">
+        <v>42453</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="22">
         <v>42450</v>
       </c>
       <c r="C9" t="s">
@@ -1113,209 +1184,640 @@
       <c r="J9" s="2">
         <v>1.5</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9" s="16">
         <v>2</v>
       </c>
-      <c r="L9" s="30"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="21">
-        <v>1</v>
-      </c>
-      <c r="B10" s="24">
+      <c r="L9" s="17"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="49">
+        <v>1</v>
+      </c>
+      <c r="B10" s="48">
         <v>42450</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="10">
         <v>6.5</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="12">
         <v>6.5</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="11">
         <v>4</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="12">
         <v>6</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="10">
         <v>5.5</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="12">
         <v>5.5</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="10">
         <v>5.5</v>
       </c>
       <c r="K10" s="3">
         <v>5.5</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="L10" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="M10" s="32"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" s="36">
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="22">
         <v>42451</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="37">
-        <v>1</v>
-      </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="37">
-        <v>1</v>
-      </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="38">
-        <v>1</v>
-      </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="38">
-        <v>1</v>
-      </c>
-      <c r="K11" s="35"/>
-      <c r="L11" s="44"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="1"/>
-    </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" s="36">
+      <c r="D11" s="23">
+        <v>1</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="23">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="24">
+        <v>1</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="24">
+        <v>1</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="18"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="22">
         <v>42451</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="45"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="29"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" s="36">
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="19">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="19">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="19">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1">
+        <v>3</v>
+      </c>
+      <c r="L12" s="15"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="22">
         <v>42451</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="45"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" s="36">
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="19">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" s="19">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="15"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+    </row>
+    <row r="14" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="22">
         <v>42451</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="45"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" s="36">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E14" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
+      <c r="H14" s="19">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="19">
+        <v>2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>2</v>
+      </c>
+      <c r="L14" s="17"/>
+    </row>
+    <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="49">
+        <v>1</v>
+      </c>
+      <c r="B15" s="48">
         <v>42451</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="45"/>
-    </row>
-    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" s="36">
-        <v>42451</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="45"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="43">
-        <v>1</v>
-      </c>
-      <c r="B17" s="40">
-        <v>42451</v>
-      </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="38"/>
+      <c r="C15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="E15" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="F15" s="11">
+        <v>7</v>
+      </c>
+      <c r="G15" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="H15" s="11">
+        <v>5</v>
+      </c>
+      <c r="I15" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="J15" s="11">
+        <v>6</v>
+      </c>
+      <c r="K15" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="47">
+        <v>1</v>
+      </c>
+      <c r="B16" s="50">
+        <v>42452</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="46">
+        <v>1</v>
+      </c>
+      <c r="E16" s="47">
+        <v>2</v>
+      </c>
+      <c r="F16" s="46">
+        <v>4</v>
+      </c>
+      <c r="G16" s="52">
+        <v>4</v>
+      </c>
+      <c r="H16" s="19">
+        <v>0</v>
+      </c>
+      <c r="I16" s="52">
+        <v>0</v>
+      </c>
+      <c r="J16" s="19">
+        <v>4</v>
+      </c>
+      <c r="K16" s="52">
+        <v>4</v>
+      </c>
+      <c r="L16" s="18"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="47">
+        <v>1</v>
+      </c>
+      <c r="B17" s="45">
+        <v>42452</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="46">
+        <v>3</v>
+      </c>
+      <c r="E17" s="47">
+        <v>4</v>
+      </c>
+      <c r="F17" s="46">
+        <v>0</v>
+      </c>
+      <c r="G17" s="47">
+        <v>0</v>
+      </c>
+      <c r="H17" s="19">
+        <v>0</v>
+      </c>
+      <c r="I17" s="47">
+        <v>0</v>
+      </c>
+      <c r="J17" s="19">
+        <v>0</v>
+      </c>
+      <c r="K17" s="47">
+        <v>0</v>
+      </c>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="47">
+        <v>1</v>
+      </c>
+      <c r="B18" s="22">
+        <v>42452</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="46">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="46">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="19">
+        <v>3</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3</v>
+      </c>
+      <c r="J18" s="19">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="49">
+        <v>1</v>
+      </c>
+      <c r="B19" s="48">
+        <v>42452</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="11">
+        <v>4</v>
+      </c>
+      <c r="E19" s="12">
+        <v>6</v>
+      </c>
+      <c r="F19" s="11">
+        <v>4</v>
+      </c>
+      <c r="G19" s="12">
+        <v>4</v>
+      </c>
+      <c r="H19" s="11">
+        <v>3</v>
+      </c>
+      <c r="I19" s="12">
+        <v>3</v>
+      </c>
+      <c r="J19" s="11">
+        <v>4</v>
+      </c>
+      <c r="K19" s="12">
+        <v>4</v>
+      </c>
+      <c r="L19" s="49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="22">
+        <v>42453</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="46">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>4</v>
+      </c>
+      <c r="F20" s="46">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="19">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="19">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="22">
+        <v>42453</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="46">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="46">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="I21" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="J21" s="19">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="22">
+        <v>42453</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="46">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="46">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1">
+        <v>3</v>
+      </c>
+      <c r="H22" s="19">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="19">
+        <v>3</v>
+      </c>
+      <c r="K22" s="1">
+        <v>3</v>
+      </c>
+      <c r="L22" s="15"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="49">
+        <v>1</v>
+      </c>
+      <c r="B23" s="48">
+        <v>42453</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="11">
+        <v>4</v>
+      </c>
+      <c r="E23" s="12">
+        <v>5</v>
+      </c>
+      <c r="F23" s="11">
+        <v>3</v>
+      </c>
+      <c r="G23" s="12">
+        <v>3</v>
+      </c>
+      <c r="H23" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="I23" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="J23" s="11">
+        <v>3</v>
+      </c>
+      <c r="K23" s="12">
+        <v>3</v>
+      </c>
+      <c r="L23" s="49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>